<commit_message>
[Improve] Add opcode RTS
</commit_message>
<xml_diff>
--- a/Sorties séquenceur.xlsx
+++ b/Sorties séquenceur.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\sysnumapp\NanoProcessor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7DF5A1-5097-4953-ADB7-C1F0388B259F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E527F273-79B9-4B9E-B61C-80E5DBDE8B14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E527F273-79B9-4B9E-B61C-80E5DBDE8B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1117,6 +1117,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1149,24 +1167,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1186,7 +1186,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1487,46 +1487,46 @@
   </sheetPr>
   <dimension ref="B1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33:G34"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="48"/>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="79"/>
-    </row>
-    <row r="3" spans="2:14" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+    </row>
+    <row r="3" spans="2:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="49" t="s">
         <v>4</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24" t="s">
         <v>1</v>
       </c>
@@ -1640,8 +1640,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="90" x14ac:dyDescent="0.3">
-      <c r="B6" s="63" t="s">
+    <row r="6" spans="2:14" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="69" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="31" t="s">
@@ -1678,8 +1678,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="36" x14ac:dyDescent="0.3">
-      <c r="B7" s="64"/>
+    <row r="7" spans="2:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="70"/>
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1715,8 +1715,8 @@
       </c>
       <c r="N7" s="38"/>
     </row>
-    <row r="8" spans="2:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="B8" s="64"/>
+    <row r="8" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B8" s="70"/>
       <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
@@ -1751,8 +1751,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="108" x14ac:dyDescent="0.3">
-      <c r="B9" s="64"/>
+    <row r="9" spans="2:14" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="70"/>
       <c r="C9" s="4" t="s">
         <v>65</v>
       </c>
@@ -1787,8 +1787,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="108" x14ac:dyDescent="0.3">
-      <c r="B10" s="64"/>
+    <row r="10" spans="2:14" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="70"/>
       <c r="C10" s="4" t="s">
         <v>66</v>
       </c>
@@ -1823,8 +1823,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="21" x14ac:dyDescent="0.3">
-      <c r="B11" s="65"/>
+    <row r="11" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B11" s="71"/>
       <c r="C11" s="55" t="s">
         <v>59</v>
       </c>
@@ -1860,8 +1860,8 @@
       </c>
       <c r="N11" s="57"/>
     </row>
-    <row r="12" spans="2:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="66"/>
+    <row r="12" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="72"/>
       <c r="C12" s="37" t="s">
         <v>36</v>
       </c>
@@ -1896,8 +1896,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.3">
-      <c r="B13" s="67" t="s">
+    <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B13" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="30" t="s">
@@ -1934,9 +1934,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="64"/>
-      <c r="C14" s="74" t="s">
+    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="70"/>
+      <c r="C14" s="68" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -1970,9 +1970,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="64"/>
-      <c r="C15" s="74"/>
+    <row r="15" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="70"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
@@ -2004,9 +2004,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="64"/>
-      <c r="C16" s="74" t="s">
+    <row r="16" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="70"/>
+      <c r="C16" s="68" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -2040,9 +2040,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="64"/>
-      <c r="C17" s="74"/>
+    <row r="17" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="70"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
@@ -2074,9 +2074,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="64"/>
-      <c r="C18" s="74" t="s">
+    <row r="18" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="70"/>
+      <c r="C18" s="68" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -2110,9 +2110,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="64"/>
-      <c r="C19" s="74"/>
+    <row r="19" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="70"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="8" t="s">
         <v>44</v>
       </c>
@@ -2144,9 +2144,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="64"/>
-      <c r="C20" s="74" t="s">
+    <row r="20" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="70"/>
+      <c r="C20" s="68" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -2180,9 +2180,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="64"/>
-      <c r="C21" s="74"/>
+    <row r="21" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="70"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="8" t="s">
         <v>44</v>
       </c>
@@ -2214,9 +2214,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="64"/>
-      <c r="C22" s="74" t="s">
+    <row r="22" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="70"/>
+      <c r="C22" s="68" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="8" t="s">
@@ -2250,9 +2250,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="64"/>
-      <c r="C23" s="74"/>
+    <row r="23" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="70"/>
+      <c r="C23" s="68"/>
       <c r="D23" s="8" t="s">
         <v>45</v>
       </c>
@@ -2284,9 +2284,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="64"/>
-      <c r="C24" s="74" t="s">
+    <row r="24" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="70"/>
+      <c r="C24" s="68" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -2320,9 +2320,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="64"/>
-      <c r="C25" s="74"/>
+    <row r="25" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="70"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="8" t="s">
         <v>45</v>
       </c>
@@ -2354,9 +2354,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="64"/>
-      <c r="C26" s="74" t="s">
+    <row r="26" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="70"/>
+      <c r="C26" s="68" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="8" t="s">
@@ -2390,9 +2390,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="64"/>
-      <c r="C27" s="74"/>
+    <row r="27" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="70"/>
+      <c r="C27" s="68"/>
       <c r="D27" s="8" t="s">
         <v>46</v>
       </c>
@@ -2424,9 +2424,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="64"/>
-      <c r="C28" s="74" t="s">
+    <row r="28" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="70"/>
+      <c r="C28" s="68" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -2460,9 +2460,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="64"/>
-      <c r="C29" s="74"/>
+    <row r="29" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="70"/>
+      <c r="C29" s="68"/>
       <c r="D29" s="8" t="s">
         <v>46</v>
       </c>
@@ -2494,8 +2494,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="64"/>
+    <row r="30" spans="2:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="70"/>
       <c r="C30" s="4" t="s">
         <v>37</v>
       </c>
@@ -2530,8 +2530,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="54" x14ac:dyDescent="0.3">
-      <c r="B31" s="64"/>
+    <row r="31" spans="2:13" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="70"/>
       <c r="C31" s="4" t="s">
         <v>47</v>
       </c>
@@ -2566,8 +2566,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="21" x14ac:dyDescent="0.3">
-      <c r="B32" s="64"/>
+    <row r="32" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="B32" s="70"/>
       <c r="C32" s="5" t="s">
         <v>38</v>
       </c>
@@ -2602,15 +2602,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="65"/>
-      <c r="C33" s="68" t="s">
+    <row r="33" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="71"/>
+      <c r="C33" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="70" t="s">
+      <c r="D33" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="72" t="s">
+      <c r="E33" s="78" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="61" t="s">
@@ -2634,15 +2634,15 @@
       <c r="L33" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="M33" s="75" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="65"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="73"/>
+      <c r="M33" s="63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="71"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="79"/>
       <c r="F34" s="62"/>
       <c r="G34" s="62"/>
       <c r="H34" s="62"/>
@@ -2650,10 +2650,10 @@
       <c r="J34" s="62"/>
       <c r="K34" s="62"/>
       <c r="L34" s="62"/>
-      <c r="M34" s="76"/>
-    </row>
-    <row r="35" spans="2:13" ht="21" x14ac:dyDescent="0.3">
-      <c r="B35" s="65"/>
+      <c r="M34" s="64"/>
+    </row>
+    <row r="35" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="B35" s="71"/>
       <c r="C35" s="55" t="s">
         <v>59</v>
       </c>
@@ -2688,8 +2688,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:13" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="66"/>
+    <row r="36" spans="2:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="72"/>
       <c r="C36" s="6" t="s">
         <v>36</v>
       </c>
@@ -2726,6 +2726,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B13:B36"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="L33:L34"/>
     <mergeCell ref="M33:M34"/>
     <mergeCell ref="E2:M2"/>
@@ -2737,17 +2743,11 @@
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="B13:B36"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
     <mergeCell ref="K33:K34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="G33:G34"/>
     <mergeCell ref="H33:H34"/>
     <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="70" orientation="portrait" r:id="rId1"/>
@@ -2762,13 +2762,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="45" t="s">
         <v>48</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="43" t="s">
         <v>50</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="39" t="s">
         <v>51</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="39" t="s">
         <v>52</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
         <v>25</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="59" t="s">
         <v>53</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="41" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
[Update] Added LOADindconst & RTS to sequencer outputs
</commit_message>
<xml_diff>
--- a/Sorties séquenceur.xlsx
+++ b/Sorties séquenceur.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\sysnumapp\NanoProcessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7DF5A1-5097-4953-ADB7-C1F0388B259F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E10D82-CBD8-4C93-95B9-90F3FADBB62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E527F273-79B9-4B9E-B61C-80E5DBDE8B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E527F273-79B9-4B9E-B61C-80E5DBDE8B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="68">
   <si>
     <t>sRESET</t>
   </si>
@@ -158,8 +158,110 @@
     <t>Autres</t>
   </si>
   <si>
+    <t>STOREaddr</t>
+  </si>
+  <si>
+    <t>Z = '0'</t>
+  </si>
+  <si>
+    <t>Z = '1'</t>
+  </si>
+  <si>
+    <t>C = '0'</t>
+  </si>
+  <si>
+    <t>V = '0'</t>
+  </si>
+  <si>
+    <t>N = '0'</t>
+  </si>
+  <si>
+    <t>C = '1'</t>
+  </si>
+  <si>
+    <t>V = '1'</t>
+  </si>
+  <si>
+    <t>N = '1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SETC
+CLRC
+TRFNC </t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Valeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUX_ACCU      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUX_CONST     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUX_DATA      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUX_ACCU_DATA </t>
+  </si>
+  <si>
+    <t>"000"</t>
+  </si>
+  <si>
+    <t>"001"</t>
+  </si>
+  <si>
+    <t>"010"</t>
+  </si>
+  <si>
+    <t>"101"</t>
+  </si>
+  <si>
+    <t>blanc</t>
+  </si>
+  <si>
+    <t>TFR</t>
+  </si>
+  <si>
+    <t>MULUconst
+MULUaddr</t>
+  </si>
+  <si>
+    <t>SecAccu_load_o</t>
+  </si>
+  <si>
+    <t>MUX_SECACCU</t>
+  </si>
+  <si>
+    <t>'"110"</t>
+  </si>
+  <si>
+    <t>"111"</t>
+  </si>
+  <si>
+    <t>ANDaddr
+Oraddr
+XORaddr
+ADDaddr
+ADCaddr
+MULUaddr</t>
+  </si>
+  <si>
+    <t>ANDconst
+Orconst
+XORconst
+ADDconst
+ADCconst
+MULUconst
+LOADindconst</t>
+  </si>
+  <si>
     <t>LOADaddr
 LOADconst
+LOADindconst
 ANDconst
 ANDaddr
 ORconst
@@ -181,104 +283,7 @@
 NEGconst</t>
   </si>
   <si>
-    <t>STOREaddr</t>
-  </si>
-  <si>
-    <t>Z = '0'</t>
-  </si>
-  <si>
-    <t>Z = '1'</t>
-  </si>
-  <si>
-    <t>C = '0'</t>
-  </si>
-  <si>
-    <t>V = '0'</t>
-  </si>
-  <si>
-    <t>N = '0'</t>
-  </si>
-  <si>
-    <t>C = '1'</t>
-  </si>
-  <si>
-    <t>V = '1'</t>
-  </si>
-  <si>
-    <t>N = '1'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SETC
-CLRC
-TRFNC </t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Valeur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUX_ACCU      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUX_CONST     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUX_DATA      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUX_ACCU_DATA </t>
-  </si>
-  <si>
-    <t>"000"</t>
-  </si>
-  <si>
-    <t>"001"</t>
-  </si>
-  <si>
-    <t>"010"</t>
-  </si>
-  <si>
-    <t>"101"</t>
-  </si>
-  <si>
-    <t>blanc</t>
-  </si>
-  <si>
-    <t>TFR</t>
-  </si>
-  <si>
-    <t>MULUconst
-MULUaddr</t>
-  </si>
-  <si>
-    <t>SecAccu_load_o</t>
-  </si>
-  <si>
-    <t>MUX_SECACCU</t>
-  </si>
-  <si>
-    <t>'"110"</t>
-  </si>
-  <si>
-    <t>"111"</t>
-  </si>
-  <si>
-    <t>ANDconst
-Orconst
-XORconst
-ADDconst
-ADCconst
-MULUconst</t>
-  </si>
-  <si>
-    <t>ANDaddr
-Oraddr
-XORaddr
-ADDaddr
-ADCaddr
-MULUaddr</t>
+    <t>RTS</t>
   </si>
 </sst>
 </file>
@@ -959,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1114,7 +1119,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1134,39 +1181,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1186,7 +1200,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1485,48 +1499,48 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N36"/>
+  <dimension ref="B1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36:J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="48"/>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-    </row>
-    <row r="3" spans="2:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="81"/>
+    </row>
+    <row r="3" spans="2:14" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="49" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="53" t="s">
         <v>6</v>
@@ -1564,7 +1578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1607,7 @@
         <v>15</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L4" s="22" t="s">
         <v>15</v>
@@ -1602,7 +1616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="24" t="s">
         <v>1</v>
       </c>
@@ -1631,7 +1645,7 @@
         <v>15</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" s="28" t="s">
         <v>15</v>
@@ -1640,8 +1654,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="69" t="s">
+    <row r="6" spans="2:14" ht="90" x14ac:dyDescent="0.3">
+      <c r="B6" s="66" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="31" t="s">
@@ -1678,8 +1692,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="70"/>
+    <row r="7" spans="2:14" ht="36" x14ac:dyDescent="0.3">
+      <c r="B7" s="67"/>
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1715,8 +1729,8 @@
       </c>
       <c r="N7" s="38"/>
     </row>
-    <row r="8" spans="2:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="B8" s="70"/>
+    <row r="8" spans="2:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="B8" s="67"/>
       <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
@@ -1751,8 +1765,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="70"/>
+    <row r="9" spans="2:14" ht="126" x14ac:dyDescent="0.3">
+      <c r="B9" s="67"/>
       <c r="C9" s="4" t="s">
         <v>65</v>
       </c>
@@ -1787,10 +1801,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="70"/>
+    <row r="10" spans="2:14" ht="108" x14ac:dyDescent="0.3">
+      <c r="B10" s="67"/>
       <c r="C10" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>18</v>
@@ -1823,10 +1837,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B11" s="71"/>
+    <row r="11" spans="2:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="B11" s="68"/>
       <c r="C11" s="55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="56" t="s">
         <v>18</v>
@@ -1850,7 +1864,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>15</v>
@@ -1860,8 +1874,8 @@
       </c>
       <c r="N11" s="57"/>
     </row>
-    <row r="12" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="72"/>
+    <row r="12" spans="2:14" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="69"/>
       <c r="C12" s="37" t="s">
         <v>36</v>
       </c>
@@ -1887,7 +1901,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>15</v>
@@ -1896,8 +1910,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B13" s="73" t="s">
+    <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="B13" s="70" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="30" t="s">
@@ -1925,7 +1939,7 @@
         <v>15</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>15</v>
@@ -1934,538 +1948,538 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="70"/>
-      <c r="C14" s="68" t="s">
+    <row r="14" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="67"/>
+      <c r="C14" s="82" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="67"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="70"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="67"/>
+      <c r="C16" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="67"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="67"/>
+      <c r="C18" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="70"/>
-      <c r="C16" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="70"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="8" t="s">
+      <c r="E18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="67"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="67"/>
+      <c r="C20" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="70"/>
-      <c r="C18" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="E20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="67"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="67"/>
+      <c r="C22" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="70"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="8" t="s">
+      <c r="E22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="67"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="70"/>
-      <c r="C20" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="E23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="67"/>
+      <c r="C24" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="70"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="8" t="s">
+      <c r="E24" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="67"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="70"/>
-      <c r="C22" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="E25" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M22" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="70"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="8" t="s">
+      <c r="E26" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="70"/>
-      <c r="C24" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="8" t="s">
+      <c r="E27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M24" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="70"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="8" t="s">
+      <c r="E28" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M25" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="70"/>
-      <c r="C26" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M26" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="70"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M27" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="70"/>
-      <c r="C28" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M28" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="70"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="E29" s="12" t="s">
         <v>15</v>
       </c>
@@ -2485,7 +2499,7 @@
         <v>15</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>15</v>
@@ -2494,10 +2508,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="70"/>
+    <row r="30" spans="2:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="67"/>
       <c r="C30" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>18</v>
@@ -2521,7 +2535,7 @@
         <v>15</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>14</v>
@@ -2530,10 +2544,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="70"/>
+    <row r="31" spans="2:13" ht="54" x14ac:dyDescent="0.3">
+      <c r="B31" s="67"/>
       <c r="C31" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>18</v>
@@ -2557,7 +2571,7 @@
         <v>15</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>14</v>
@@ -2566,10 +2580,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="B32" s="70"/>
+    <row r="32" spans="2:13" ht="21" x14ac:dyDescent="0.3">
+      <c r="B32" s="67"/>
       <c r="C32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>18</v>
@@ -2593,7 +2607,7 @@
         <v>15</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>14</v>
@@ -2602,60 +2616,60 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="71"/>
-      <c r="C33" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="76" t="s">
+    <row r="33" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="68"/>
+      <c r="C33" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="J33" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="K33" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="L33" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="M33" s="63" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="71"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="62"/>
-      <c r="M34" s="64"/>
-    </row>
-    <row r="35" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="B35" s="71"/>
+      <c r="E33" s="75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="L33" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="68"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="78"/>
+    </row>
+    <row r="35" spans="2:13" ht="21" x14ac:dyDescent="0.3">
+      <c r="B35" s="68"/>
       <c r="C35" s="55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="56" t="s">
         <v>18</v>
@@ -2667,7 +2681,7 @@
         <v>15</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>15</v>
@@ -2679,7 +2693,7 @@
         <v>15</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>14</v>
@@ -2688,50 +2702,68 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="72"/>
-      <c r="C36" s="6" t="s">
+    <row r="36" spans="2:13" ht="21" x14ac:dyDescent="0.3">
+      <c r="B36" s="68"/>
+      <c r="C36" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="63"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L36" s="61"/>
+      <c r="M36" s="62"/>
+    </row>
+    <row r="37" spans="2:13" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="69"/>
+      <c r="C37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L36" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M36" s="16" t="s">
+      <c r="E37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L37" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M37" s="16" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="B13:B36"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
     <mergeCell ref="L33:L34"/>
     <mergeCell ref="M33:M34"/>
     <mergeCell ref="E2:M2"/>
@@ -2748,6 +2780,12 @@
     <mergeCell ref="G33:G34"/>
     <mergeCell ref="H33:H34"/>
     <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B13:B37"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="70" orientation="portrait" r:id="rId1"/>
@@ -2762,66 +2800,66 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="45" t="s">
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="43" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="C3" s="44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C4" s="40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C5" s="40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="42" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>